<commit_message>
Included All Issue Reason
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteDOCS/testdata/DocumentRegistryTestData-Newtransmittal.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteDOCS/testdata/DocumentRegistryTestData-Newtransmittal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>To</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>AutoTestUser</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Comments for Request for Information</t>
+  </si>
+  <si>
+    <t>Request for Information</t>
+  </si>
+  <si>
+    <t>Issued for Approval</t>
+  </si>
+  <si>
+    <t>Issued for Information</t>
   </si>
 </sst>
 </file>
@@ -491,7 +506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -579,7 +594,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -587,8 +602,92 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>